<commit_message>
Projeto de Teste - Exclusão, Browser e Tags
Correção da UC005 do Projeto de Teste - Exclusão, Browser e Tags
</commit_message>
<xml_diff>
--- a/Projeto de Teste - Exclusão, Browsers e Tags.xlsx
+++ b/Projeto de Teste - Exclusão, Browsers e Tags.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" codeName="EstaPasta_de_trabalho" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="601" activeTab="3"/>
+    <workbookView xWindow="1215" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="601" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="164">
   <si>
     <t>CAMPO</t>
   </si>
@@ -1083,6 +1083,28 @@
       <t>Tela Principal</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Selecionar </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Livro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> a ser associado uma ou mais Tags</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1727,6 +1749,27 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1784,39 +1827,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1841,6 +1851,18 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1851,691 +1873,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="170">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
+  <dxfs count="94">
     <dxf>
       <font>
         <b/>
@@ -4240,20 +3578,20 @@
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="77" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="93"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="60" t="s">
         <v>10</v>
       </c>
@@ -4488,23 +3826,23 @@
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="74" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="I2" s="93"/>
-      <c r="J2" s="90" t="s">
+      <c r="I2" s="74"/>
+      <c r="J2" s="71" t="s">
         <v>100</v>
       </c>
       <c r="K2" s="38"/>
@@ -4735,20 +4073,20 @@
       <c r="IB2" s="1"/>
     </row>
     <row r="3" spans="1:236" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="72"/>
       <c r="K3" s="38"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -4977,16 +4315,16 @@
       <c r="IB3" s="1"/>
     </row>
     <row r="4" spans="1:236" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="96"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="92"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="73"/>
       <c r="K4" s="38"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -6437,13 +5775,13 @@
       <c r="IB9" s="1"/>
     </row>
     <row r="10" spans="1:236" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="71">
+      <c r="A10" s="78">
         <v>2</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="80" t="s">
         <v>138</v>
       </c>
       <c r="D10" s="62" t="s">
@@ -6687,9 +6025,9 @@
       <c r="IB10" s="13"/>
     </row>
     <row r="11" spans="1:236" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="62" t="s">
         <v>140</v>
       </c>
@@ -7419,13 +6757,13 @@
       <c r="IB13" s="1"/>
     </row>
     <row r="14" spans="1:236" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="71">
+      <c r="A14" s="78">
         <v>3</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="80" t="s">
         <v>138</v>
       </c>
       <c r="D14" s="62" t="s">
@@ -7669,9 +7007,9 @@
       <c r="IB14" s="13"/>
     </row>
     <row r="15" spans="1:236" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="62" t="s">
         <v>141</v>
       </c>
@@ -8167,13 +7505,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="G2:G4"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -8184,13 +7515,20 @@
     <mergeCell ref="B3:D4"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="G2:G4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="F7 J6:J7 H6">
     <cfRule type="cellIs" priority="271" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="272" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="272" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8198,7 +7536,7 @@
     <cfRule type="cellIs" priority="241" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="242" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8206,7 +7544,7 @@
     <cfRule type="cellIs" priority="77" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="78" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8214,7 +7552,7 @@
     <cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="18" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8222,7 +7560,7 @@
     <cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="16" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8230,7 +7568,7 @@
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="14" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8238,7 +7576,7 @@
     <cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="12" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8246,7 +7584,7 @@
     <cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="10" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8254,7 +7592,7 @@
     <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="8" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8262,7 +7600,7 @@
     <cfRule type="cellIs" priority="5" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="6" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8270,7 +7608,7 @@
     <cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="4" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8278,7 +7616,7 @@
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="2" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8300,11 +7638,11 @@
   <sheetPr codeName="Plan6"/>
   <dimension ref="A1:II104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8328,30 +7666,30 @@
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="77" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="105" t="s">
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="107"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+      <c r="Q1" s="103"/>
       <c r="R1" s="38"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -8583,44 +7921,44 @@
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="74" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="81" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="81" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="J2" s="74" t="s">
+      <c r="J2" s="81" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="74" t="s">
+      <c r="K2" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="L2" s="74" t="s">
+      <c r="L2" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="M2" s="93"/>
-      <c r="N2" s="90" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="101" t="s">
+      <c r="O2" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="101" t="s">
+      <c r="P2" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="101" t="s">
+      <c r="Q2" s="97" t="s">
         <v>39</v>
       </c>
       <c r="R2" s="38"/>
@@ -8851,27 +8189,27 @@
       <c r="II2" s="1"/>
     </row>
     <row r="3" spans="1:243" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="102"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
       <c r="R3" s="38"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -9100,23 +8438,23 @@
       <c r="II3" s="1"/>
     </row>
     <row r="4" spans="1:243" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="96"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="103"/>
-      <c r="P4" s="103"/>
-      <c r="Q4" s="103"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
       <c r="R4" s="38"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -9845,13 +9183,13 @@
       <c r="II6" s="1"/>
     </row>
     <row r="7" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="71">
+      <c r="A7" s="78">
         <v>1</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="80" t="s">
         <v>112</v>
       </c>
       <c r="D7" s="63" t="s">
@@ -10102,9 +9440,9 @@
       <c r="II7" s="13"/>
     </row>
     <row r="8" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="71"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="63" t="s">
         <v>46</v>
       </c>
@@ -10351,9 +9689,9 @@
       <c r="II8" s="13"/>
     </row>
     <row r="9" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="63" t="s">
         <v>48</v>
       </c>
@@ -10847,13 +10185,13 @@
       <c r="II10"/>
     </row>
     <row r="11" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="80" t="s">
         <v>112</v>
       </c>
       <c r="D11" s="63" t="s">
@@ -11102,9 +10440,9 @@
       <c r="II11" s="13"/>
     </row>
     <row r="12" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="71"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="63" t="s">
         <v>46</v>
       </c>
@@ -11361,9 +10699,9 @@
       <c r="II12" s="13"/>
     </row>
     <row r="13" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="71"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="63" t="s">
         <v>48</v>
       </c>
@@ -11616,9 +10954,9 @@
       <c r="II13" s="13"/>
     </row>
     <row r="14" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="71"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="63" t="s">
         <v>46</v>
       </c>
@@ -11875,9 +11213,9 @@
       <c r="II14" s="13"/>
     </row>
     <row r="15" spans="1:243" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="72"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="63" t="s">
         <v>48</v>
       </c>
@@ -12375,13 +11713,13 @@
       <c r="II16"/>
     </row>
     <row r="17" spans="1:243" s="9" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="71">
+      <c r="A17" s="78">
         <v>3</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="106" t="s">
         <v>112</v>
       </c>
       <c r="D17" s="48" t="s">
@@ -12630,9 +11968,9 @@
       <c r="II17" s="13"/>
     </row>
     <row r="18" spans="1:243" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="71"/>
-      <c r="B18" s="98"/>
-      <c r="C18" s="98"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="107"/>
+      <c r="C18" s="107"/>
       <c r="D18" s="48" t="s">
         <v>46</v>
       </c>
@@ -12889,9 +12227,9 @@
       <c r="II18" s="13"/>
     </row>
     <row r="19" spans="1:243" s="9" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="98"/>
-      <c r="C19" s="98"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="107"/>
       <c r="D19" s="48" t="s">
         <v>48</v>
       </c>
@@ -13387,13 +12725,13 @@
       <c r="II20"/>
     </row>
     <row r="21" spans="1:243" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="71">
+      <c r="A21" s="78">
         <v>4</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="98" t="s">
+      <c r="C21" s="107" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="48" t="s">
@@ -13642,9 +12980,9 @@
       <c r="II21" s="13"/>
     </row>
     <row r="22" spans="1:243" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="71"/>
-      <c r="B22" s="98"/>
-      <c r="C22" s="98"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="107"/>
       <c r="D22" s="48" t="s">
         <v>46</v>
       </c>
@@ -13901,9 +13239,9 @@
       <c r="II22" s="13"/>
     </row>
     <row r="23" spans="1:243" s="9" customFormat="1" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="107"/>
       <c r="D23" s="48" t="s">
         <v>48</v>
       </c>
@@ -14405,13 +13743,13 @@
       <c r="II24"/>
     </row>
     <row r="25" spans="1:243" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="97" t="s">
+      <c r="A25" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="98" t="s">
+      <c r="C25" s="107" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="48" t="s">
@@ -14435,9 +13773,9 @@
       <c r="R25" s="38"/>
     </row>
     <row r="26" spans="1:243" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="71"/>
-      <c r="B26" s="98"/>
-      <c r="C26" s="98"/>
+      <c r="A26" s="78"/>
+      <c r="B26" s="107"/>
+      <c r="C26" s="107"/>
       <c r="D26" s="48" t="s">
         <v>46</v>
       </c>
@@ -14469,9 +13807,9 @@
       <c r="R26" s="38"/>
     </row>
     <row r="27" spans="1:243" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
-      <c r="B27" s="98"/>
-      <c r="C27" s="98"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="107"/>
+      <c r="C27" s="107"/>
       <c r="D27" s="48" t="s">
         <v>48</v>
       </c>
@@ -14517,13 +13855,13 @@
       <c r="R28" s="58"/>
     </row>
     <row r="29" spans="1:243" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="97" t="s">
+      <c r="A29" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="98" t="s">
+      <c r="C29" s="107" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="48" t="s">
@@ -14547,9 +13885,9 @@
       <c r="R29" s="38"/>
     </row>
     <row r="30" spans="1:243" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="71"/>
-      <c r="B30" s="98"/>
-      <c r="C30" s="98"/>
+      <c r="A30" s="78"/>
+      <c r="B30" s="107"/>
+      <c r="C30" s="107"/>
       <c r="D30" s="48" t="s">
         <v>46</v>
       </c>
@@ -14581,9 +13919,9 @@
       <c r="R30" s="38"/>
     </row>
     <row r="31" spans="1:243" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="71"/>
-      <c r="B31" s="98"/>
-      <c r="C31" s="98"/>
+      <c r="A31" s="78"/>
+      <c r="B31" s="107"/>
+      <c r="C31" s="107"/>
       <c r="D31" s="48" t="s">
         <v>48</v>
       </c>
@@ -14631,13 +13969,13 @@
       <c r="R32" s="58"/>
     </row>
     <row r="33" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="97" t="s">
+      <c r="A33" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="98" t="s">
+      <c r="C33" s="107" t="s">
         <v>33</v>
       </c>
       <c r="D33" s="48" t="s">
@@ -14661,9 +13999,9 @@
       <c r="R33" s="38"/>
     </row>
     <row r="34" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="71"/>
-      <c r="B34" s="98"/>
-      <c r="C34" s="98"/>
+      <c r="A34" s="78"/>
+      <c r="B34" s="107"/>
+      <c r="C34" s="107"/>
       <c r="D34" s="48" t="s">
         <v>46</v>
       </c>
@@ -14695,9 +14033,9 @@
       <c r="R34" s="38"/>
     </row>
     <row r="35" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="71"/>
-      <c r="B35" s="98"/>
-      <c r="C35" s="98"/>
+      <c r="A35" s="78"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="107"/>
       <c r="D35" s="48" t="s">
         <v>48</v>
       </c>
@@ -14743,13 +14081,13 @@
       <c r="R36" s="58"/>
     </row>
     <row r="37" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="97" t="s">
+      <c r="A37" s="108" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="98" t="s">
+      <c r="B37" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="98" t="s">
+      <c r="C37" s="107" t="s">
         <v>35</v>
       </c>
       <c r="D37" s="48" t="s">
@@ -14773,9 +14111,9 @@
       <c r="R37" s="38"/>
     </row>
     <row r="38" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="71"/>
-      <c r="B38" s="98"/>
-      <c r="C38" s="98"/>
+      <c r="A38" s="78"/>
+      <c r="B38" s="107"/>
+      <c r="C38" s="107"/>
       <c r="D38" s="48" t="s">
         <v>46</v>
       </c>
@@ -14807,9 +14145,9 @@
       <c r="R38" s="38"/>
     </row>
     <row r="39" spans="1:18" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
-      <c r="B39" s="98"/>
-      <c r="C39" s="98"/>
+      <c r="A39" s="78"/>
+      <c r="B39" s="107"/>
+      <c r="C39" s="107"/>
       <c r="D39" s="48" t="s">
         <v>48</v>
       </c>
@@ -14861,13 +14199,13 @@
       <c r="R40" s="58"/>
     </row>
     <row r="41" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="97" t="s">
+      <c r="A41" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="98" t="s">
+      <c r="C41" s="107" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="48" t="s">
@@ -14891,9 +14229,9 @@
       <c r="R41" s="38"/>
     </row>
     <row r="42" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="71"/>
-      <c r="B42" s="98"/>
-      <c r="C42" s="98"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="107"/>
+      <c r="C42" s="107"/>
       <c r="D42" s="48" t="s">
         <v>46</v>
       </c>
@@ -14925,9 +14263,9 @@
       <c r="R42" s="38"/>
     </row>
     <row r="43" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
-      <c r="B43" s="98"/>
-      <c r="C43" s="98"/>
+      <c r="A43" s="78"/>
+      <c r="B43" s="107"/>
+      <c r="C43" s="107"/>
       <c r="D43" s="48" t="s">
         <v>48</v>
       </c>
@@ -14973,13 +14311,13 @@
       <c r="R44" s="58"/>
     </row>
     <row r="45" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="97" t="s">
+      <c r="A45" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="98" t="s">
+      <c r="C45" s="107" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="48" t="s">
@@ -15003,9 +14341,9 @@
       <c r="R45" s="38"/>
     </row>
     <row r="46" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="71"/>
-      <c r="B46" s="98"/>
-      <c r="C46" s="98"/>
+      <c r="A46" s="78"/>
+      <c r="B46" s="107"/>
+      <c r="C46" s="107"/>
       <c r="D46" s="48" t="s">
         <v>46</v>
       </c>
@@ -15037,9 +14375,9 @@
       <c r="R46" s="38"/>
     </row>
     <row r="47" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="71"/>
-      <c r="B47" s="98"/>
-      <c r="C47" s="98"/>
+      <c r="A47" s="78"/>
+      <c r="B47" s="107"/>
+      <c r="C47" s="107"/>
       <c r="D47" s="48" t="s">
         <v>48</v>
       </c>
@@ -15087,13 +14425,13 @@
       <c r="R48" s="58"/>
     </row>
     <row r="49" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="97" t="s">
+      <c r="A49" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="98" t="s">
+      <c r="B49" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="98" t="s">
+      <c r="C49" s="107" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="48" t="s">
@@ -15117,9 +14455,9 @@
       <c r="R49" s="38"/>
     </row>
     <row r="50" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="71"/>
-      <c r="B50" s="98"/>
-      <c r="C50" s="98"/>
+      <c r="A50" s="78"/>
+      <c r="B50" s="107"/>
+      <c r="C50" s="107"/>
       <c r="D50" s="48" t="s">
         <v>46</v>
       </c>
@@ -15151,9 +14489,9 @@
       <c r="R50" s="38"/>
     </row>
     <row r="51" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="71"/>
-      <c r="B51" s="98"/>
-      <c r="C51" s="98"/>
+      <c r="A51" s="78"/>
+      <c r="B51" s="107"/>
+      <c r="C51" s="107"/>
       <c r="D51" s="48" t="s">
         <v>48</v>
       </c>
@@ -15199,13 +14537,13 @@
       <c r="R52" s="58"/>
     </row>
     <row r="53" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="97" t="s">
+      <c r="A53" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="B53" s="98" t="s">
+      <c r="B53" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="98" t="s">
+      <c r="C53" s="107" t="s">
         <v>35</v>
       </c>
       <c r="D53" s="48" t="s">
@@ -15229,9 +14567,9 @@
       <c r="R53" s="38"/>
     </row>
     <row r="54" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="71"/>
-      <c r="B54" s="98"/>
-      <c r="C54" s="98"/>
+      <c r="A54" s="78"/>
+      <c r="B54" s="107"/>
+      <c r="C54" s="107"/>
       <c r="D54" s="48" t="s">
         <v>46</v>
       </c>
@@ -15263,9 +14601,9 @@
       <c r="R54" s="38"/>
     </row>
     <row r="55" spans="1:18" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="71"/>
-      <c r="B55" s="98"/>
-      <c r="C55" s="98"/>
+      <c r="A55" s="78"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="107"/>
       <c r="D55" s="48" t="s">
         <v>48</v>
       </c>
@@ -15317,13 +14655,13 @@
       <c r="R56" s="58"/>
     </row>
     <row r="57" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="97" t="s">
+      <c r="A57" s="108" t="s">
         <v>77</v>
       </c>
-      <c r="B57" s="98" t="s">
+      <c r="B57" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="98" t="s">
+      <c r="C57" s="107" t="s">
         <v>16</v>
       </c>
       <c r="D57" s="48" t="s">
@@ -15347,9 +14685,9 @@
       <c r="R57" s="38"/>
     </row>
     <row r="58" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="71"/>
-      <c r="B58" s="98"/>
-      <c r="C58" s="98"/>
+      <c r="A58" s="78"/>
+      <c r="B58" s="107"/>
+      <c r="C58" s="107"/>
       <c r="D58" s="48" t="s">
         <v>46</v>
       </c>
@@ -15381,9 +14719,9 @@
       <c r="R58" s="38"/>
     </row>
     <row r="59" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="71"/>
-      <c r="B59" s="98"/>
-      <c r="C59" s="98"/>
+      <c r="A59" s="78"/>
+      <c r="B59" s="107"/>
+      <c r="C59" s="107"/>
       <c r="D59" s="48" t="s">
         <v>48</v>
       </c>
@@ -15429,13 +14767,13 @@
       <c r="R60" s="58"/>
     </row>
     <row r="61" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A61" s="97" t="s">
+      <c r="A61" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="98" t="s">
+      <c r="B61" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="98" t="s">
+      <c r="C61" s="107" t="s">
         <v>17</v>
       </c>
       <c r="D61" s="48" t="s">
@@ -15459,9 +14797,9 @@
       <c r="R61" s="38"/>
     </row>
     <row r="62" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A62" s="71"/>
-      <c r="B62" s="98"/>
-      <c r="C62" s="98"/>
+      <c r="A62" s="78"/>
+      <c r="B62" s="107"/>
+      <c r="C62" s="107"/>
       <c r="D62" s="48" t="s">
         <v>46</v>
       </c>
@@ -15493,9 +14831,9 @@
       <c r="R62" s="38"/>
     </row>
     <row r="63" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="71"/>
-      <c r="B63" s="98"/>
-      <c r="C63" s="98"/>
+      <c r="A63" s="78"/>
+      <c r="B63" s="107"/>
+      <c r="C63" s="107"/>
       <c r="D63" s="48" t="s">
         <v>48</v>
       </c>
@@ -15543,13 +14881,13 @@
       <c r="R64" s="58"/>
     </row>
     <row r="65" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="97" t="s">
+      <c r="A65" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="98" t="s">
+      <c r="B65" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="98" t="s">
+      <c r="C65" s="107" t="s">
         <v>33</v>
       </c>
       <c r="D65" s="48" t="s">
@@ -15573,9 +14911,9 @@
       <c r="R65" s="38"/>
     </row>
     <row r="66" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A66" s="71"/>
-      <c r="B66" s="98"/>
-      <c r="C66" s="98"/>
+      <c r="A66" s="78"/>
+      <c r="B66" s="107"/>
+      <c r="C66" s="107"/>
       <c r="D66" s="48" t="s">
         <v>46</v>
       </c>
@@ -15607,9 +14945,9 @@
       <c r="R66" s="38"/>
     </row>
     <row r="67" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="71"/>
-      <c r="B67" s="98"/>
-      <c r="C67" s="98"/>
+      <c r="A67" s="78"/>
+      <c r="B67" s="107"/>
+      <c r="C67" s="107"/>
       <c r="D67" s="48" t="s">
         <v>48</v>
       </c>
@@ -15655,13 +14993,13 @@
       <c r="R68" s="58"/>
     </row>
     <row r="69" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A69" s="97" t="s">
+      <c r="A69" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="B69" s="98" t="s">
+      <c r="B69" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C69" s="98" t="s">
+      <c r="C69" s="107" t="s">
         <v>35</v>
       </c>
       <c r="D69" s="48" t="s">
@@ -15685,9 +15023,9 @@
       <c r="R69" s="38"/>
     </row>
     <row r="70" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A70" s="71"/>
-      <c r="B70" s="98"/>
-      <c r="C70" s="98"/>
+      <c r="A70" s="78"/>
+      <c r="B70" s="107"/>
+      <c r="C70" s="107"/>
       <c r="D70" s="48" t="s">
         <v>46</v>
       </c>
@@ -15719,9 +15057,9 @@
       <c r="R70" s="38"/>
     </row>
     <row r="71" spans="1:18" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="71"/>
-      <c r="B71" s="98"/>
-      <c r="C71" s="98"/>
+      <c r="A71" s="78"/>
+      <c r="B71" s="107"/>
+      <c r="C71" s="107"/>
       <c r="D71" s="48" t="s">
         <v>48</v>
       </c>
@@ -15773,13 +15111,13 @@
       <c r="R72" s="58"/>
     </row>
     <row r="73" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A73" s="97" t="s">
+      <c r="A73" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="B73" s="98" t="s">
+      <c r="B73" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="98" t="s">
+      <c r="C73" s="107" t="s">
         <v>16</v>
       </c>
       <c r="D73" s="48" t="s">
@@ -15803,9 +15141,9 @@
       <c r="R73" s="38"/>
     </row>
     <row r="74" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="71"/>
-      <c r="B74" s="98"/>
-      <c r="C74" s="98"/>
+      <c r="A74" s="78"/>
+      <c r="B74" s="107"/>
+      <c r="C74" s="107"/>
       <c r="D74" s="48" t="s">
         <v>46</v>
       </c>
@@ -15837,9 +15175,9 @@
       <c r="R74" s="38"/>
     </row>
     <row r="75" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="71"/>
-      <c r="B75" s="98"/>
-      <c r="C75" s="98"/>
+      <c r="A75" s="78"/>
+      <c r="B75" s="107"/>
+      <c r="C75" s="107"/>
       <c r="D75" s="48" t="s">
         <v>48</v>
       </c>
@@ -15885,13 +15223,13 @@
       <c r="R76" s="58"/>
     </row>
     <row r="77" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A77" s="97" t="s">
+      <c r="A77" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="B77" s="98" t="s">
+      <c r="B77" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="98" t="s">
+      <c r="C77" s="107" t="s">
         <v>17</v>
       </c>
       <c r="D77" s="48" t="s">
@@ -15915,9 +15253,9 @@
       <c r="R77" s="38"/>
     </row>
     <row r="78" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A78" s="71"/>
-      <c r="B78" s="98"/>
-      <c r="C78" s="98"/>
+      <c r="A78" s="78"/>
+      <c r="B78" s="107"/>
+      <c r="C78" s="107"/>
       <c r="D78" s="48" t="s">
         <v>46</v>
       </c>
@@ -15949,9 +15287,9 @@
       <c r="R78" s="38"/>
     </row>
     <row r="79" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="71"/>
-      <c r="B79" s="98"/>
-      <c r="C79" s="98"/>
+      <c r="A79" s="78"/>
+      <c r="B79" s="107"/>
+      <c r="C79" s="107"/>
       <c r="D79" s="48" t="s">
         <v>48</v>
       </c>
@@ -15999,13 +15337,13 @@
       <c r="R80" s="58"/>
     </row>
     <row r="81" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A81" s="97" t="s">
+      <c r="A81" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="B81" s="98" t="s">
+      <c r="B81" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="98" t="s">
+      <c r="C81" s="107" t="s">
         <v>33</v>
       </c>
       <c r="D81" s="48" t="s">
@@ -16029,9 +15367,9 @@
       <c r="R81" s="38"/>
     </row>
     <row r="82" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="71"/>
-      <c r="B82" s="98"/>
-      <c r="C82" s="98"/>
+      <c r="A82" s="78"/>
+      <c r="B82" s="107"/>
+      <c r="C82" s="107"/>
       <c r="D82" s="48" t="s">
         <v>46</v>
       </c>
@@ -16063,9 +15401,9 @@
       <c r="R82" s="38"/>
     </row>
     <row r="83" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="71"/>
-      <c r="B83" s="98"/>
-      <c r="C83" s="98"/>
+      <c r="A83" s="78"/>
+      <c r="B83" s="107"/>
+      <c r="C83" s="107"/>
       <c r="D83" s="48" t="s">
         <v>48</v>
       </c>
@@ -16111,13 +15449,13 @@
       <c r="R84" s="58"/>
     </row>
     <row r="85" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A85" s="97" t="s">
+      <c r="A85" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="98" t="s">
+      <c r="B85" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C85" s="98" t="s">
+      <c r="C85" s="107" t="s">
         <v>35</v>
       </c>
       <c r="D85" s="48" t="s">
@@ -16141,9 +15479,9 @@
       <c r="R85" s="38"/>
     </row>
     <row r="86" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A86" s="71"/>
-      <c r="B86" s="98"/>
-      <c r="C86" s="98"/>
+      <c r="A86" s="78"/>
+      <c r="B86" s="107"/>
+      <c r="C86" s="107"/>
       <c r="D86" s="48" t="s">
         <v>46</v>
       </c>
@@ -16175,9 +15513,9 @@
       <c r="R86" s="38"/>
     </row>
     <row r="87" spans="1:18" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="71"/>
-      <c r="B87" s="98"/>
-      <c r="C87" s="98"/>
+      <c r="A87" s="78"/>
+      <c r="B87" s="107"/>
+      <c r="C87" s="107"/>
       <c r="D87" s="48" t="s">
         <v>48</v>
       </c>
@@ -16229,13 +15567,13 @@
       <c r="R88" s="58"/>
     </row>
     <row r="89" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A89" s="97" t="s">
+      <c r="A89" s="108" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="98" t="s">
+      <c r="B89" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C89" s="98" t="s">
+      <c r="C89" s="107" t="s">
         <v>16</v>
       </c>
       <c r="D89" s="48" t="s">
@@ -16259,9 +15597,9 @@
       <c r="R89" s="38"/>
     </row>
     <row r="90" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="71"/>
-      <c r="B90" s="98"/>
-      <c r="C90" s="98"/>
+      <c r="A90" s="78"/>
+      <c r="B90" s="107"/>
+      <c r="C90" s="107"/>
       <c r="D90" s="48" t="s">
         <v>46</v>
       </c>
@@ -16293,9 +15631,9 @@
       <c r="R90" s="38"/>
     </row>
     <row r="91" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="71"/>
-      <c r="B91" s="98"/>
-      <c r="C91" s="98"/>
+      <c r="A91" s="78"/>
+      <c r="B91" s="107"/>
+      <c r="C91" s="107"/>
       <c r="D91" s="48" t="s">
         <v>48</v>
       </c>
@@ -16341,13 +15679,13 @@
       <c r="R92" s="58"/>
     </row>
     <row r="93" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="97" t="s">
+      <c r="A93" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="B93" s="98" t="s">
+      <c r="B93" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="C93" s="98" t="s">
+      <c r="C93" s="107" t="s">
         <v>17</v>
       </c>
       <c r="D93" s="48" t="s">
@@ -16371,9 +15709,9 @@
       <c r="R93" s="38"/>
     </row>
     <row r="94" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="71"/>
-      <c r="B94" s="98"/>
-      <c r="C94" s="98"/>
+      <c r="A94" s="78"/>
+      <c r="B94" s="107"/>
+      <c r="C94" s="107"/>
       <c r="D94" s="48" t="s">
         <v>46</v>
       </c>
@@ -16405,9 +15743,9 @@
       <c r="R94" s="38"/>
     </row>
     <row r="95" spans="1:18" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="71"/>
-      <c r="B95" s="98"/>
-      <c r="C95" s="98"/>
+      <c r="A95" s="78"/>
+      <c r="B95" s="107"/>
+      <c r="C95" s="107"/>
       <c r="D95" s="48" t="s">
         <v>48</v>
       </c>
@@ -16455,13 +15793,13 @@
       <c r="R96" s="58"/>
     </row>
     <row r="97" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="97" t="s">
+      <c r="A97" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="B97" s="98" t="s">
+      <c r="B97" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="C97" s="98" t="s">
+      <c r="C97" s="107" t="s">
         <v>33</v>
       </c>
       <c r="D97" s="48" t="s">
@@ -16485,9 +15823,9 @@
       <c r="R97" s="38"/>
     </row>
     <row r="98" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A98" s="71"/>
-      <c r="B98" s="98"/>
-      <c r="C98" s="98"/>
+      <c r="A98" s="78"/>
+      <c r="B98" s="107"/>
+      <c r="C98" s="107"/>
       <c r="D98" s="48" t="s">
         <v>46</v>
       </c>
@@ -16519,9 +15857,9 @@
       <c r="R98" s="38"/>
     </row>
     <row r="99" spans="1:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="71"/>
-      <c r="B99" s="98"/>
-      <c r="C99" s="98"/>
+      <c r="A99" s="78"/>
+      <c r="B99" s="107"/>
+      <c r="C99" s="107"/>
       <c r="D99" s="48" t="s">
         <v>48</v>
       </c>
@@ -16567,13 +15905,13 @@
       <c r="R100" s="58"/>
     </row>
     <row r="101" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A101" s="97" t="s">
+      <c r="A101" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="B101" s="98" t="s">
+      <c r="B101" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C101" s="98" t="s">
+      <c r="C101" s="107" t="s">
         <v>35</v>
       </c>
       <c r="D101" s="48" t="s">
@@ -16597,9 +15935,9 @@
       <c r="R101" s="38"/>
     </row>
     <row r="102" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A102" s="71"/>
-      <c r="B102" s="98"/>
-      <c r="C102" s="98"/>
+      <c r="A102" s="78"/>
+      <c r="B102" s="107"/>
+      <c r="C102" s="107"/>
       <c r="D102" s="48" t="s">
         <v>46</v>
       </c>
@@ -16631,9 +15969,9 @@
       <c r="R102" s="38"/>
     </row>
     <row r="103" spans="1:18" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="71"/>
-      <c r="B103" s="98"/>
-      <c r="C103" s="98"/>
+      <c r="A103" s="78"/>
+      <c r="B103" s="107"/>
+      <c r="C103" s="107"/>
       <c r="D103" s="48" t="s">
         <v>48</v>
       </c>
@@ -16686,6 +16024,82 @@
     </row>
   </sheetData>
   <mergeCells count="91">
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="A93:A95"/>
+    <mergeCell ref="B93:B95"/>
+    <mergeCell ref="C93:C95"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="C85:C87"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="C73:C75"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
     <mergeCell ref="P2:P4"/>
@@ -16701,88 +16115,12 @@
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="J2:J4"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="C73:C75"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="A93:A95"/>
-    <mergeCell ref="B93:B95"/>
-    <mergeCell ref="C93:C95"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="C101:C103"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F9 G6:L6 N6:Q9 F25:F27 F41:F43 F57:F59 F73:F75 F89:F91 N25:Q27 N41:Q43 N57:Q59 N73:Q75 N89:Q91">
     <cfRule type="cellIs" priority="91" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="92" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16790,7 +16128,7 @@
     <cfRule type="cellIs" priority="89" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="90" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16798,7 +16136,7 @@
     <cfRule type="cellIs" priority="87" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="88" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16806,7 +16144,7 @@
     <cfRule type="cellIs" priority="85" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="86" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16814,7 +16152,7 @@
     <cfRule type="cellIs" priority="83" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="84" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16822,7 +16160,7 @@
     <cfRule type="cellIs" priority="81" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="82" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16830,7 +16168,7 @@
     <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="80" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16838,7 +16176,7 @@
     <cfRule type="cellIs" priority="77" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="78" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16846,7 +16184,7 @@
     <cfRule type="cellIs" priority="75" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="76" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16854,7 +16192,7 @@
     <cfRule type="cellIs" priority="73" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="74" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16862,7 +16200,7 @@
     <cfRule type="cellIs" priority="71" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="72" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16870,7 +16208,7 @@
     <cfRule type="cellIs" priority="69" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="70" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16878,7 +16216,7 @@
     <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="68" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16886,7 +16224,7 @@
     <cfRule type="cellIs" priority="65" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="66" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16894,7 +16232,7 @@
     <cfRule type="cellIs" priority="63" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="64" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16902,7 +16240,7 @@
     <cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="62" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16910,7 +16248,7 @@
     <cfRule type="cellIs" priority="59" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="60" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16918,7 +16256,7 @@
     <cfRule type="cellIs" priority="57" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="58" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16926,7 +16264,7 @@
     <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="56" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16934,7 +16272,7 @@
     <cfRule type="cellIs" priority="53" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="54" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16942,7 +16280,7 @@
     <cfRule type="cellIs" priority="51" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="52" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16950,7 +16288,7 @@
     <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="50" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16958,7 +16296,7 @@
     <cfRule type="cellIs" priority="47" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="48" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16966,7 +16304,7 @@
     <cfRule type="cellIs" priority="45" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="46" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16974,7 +16312,7 @@
     <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="44" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16982,7 +16320,7 @@
     <cfRule type="cellIs" priority="41" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="42" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16990,7 +16328,7 @@
     <cfRule type="cellIs" priority="39" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="40" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16998,7 +16336,7 @@
     <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="38" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17006,7 +16344,7 @@
     <cfRule type="cellIs" priority="35" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="36" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17014,7 +16352,7 @@
     <cfRule type="cellIs" priority="33" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="34" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17022,7 +16360,7 @@
     <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="20" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17030,7 +16368,7 @@
     <cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="18" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17038,7 +16376,7 @@
     <cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="16" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17046,7 +16384,7 @@
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="14" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17054,7 +16392,7 @@
     <cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="12" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17062,7 +16400,7 @@
     <cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="10" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17070,7 +16408,7 @@
     <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17078,7 +16416,7 @@
     <cfRule type="cellIs" priority="5" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="6" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17086,7 +16424,7 @@
     <cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="4" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17094,7 +16432,7 @@
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="2" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17111,11 +16449,11 @@
   <sheetPr codeName="Plan5"/>
   <dimension ref="A1:IC20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17138,21 +16476,21 @@
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="77" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="93"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="74"/>
       <c r="K1" s="60" t="s">
         <v>10</v>
       </c>
@@ -17387,26 +16725,26 @@
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="74" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="93"/>
-      <c r="K2" s="90" t="s">
+      <c r="J2" s="74"/>
+      <c r="K2" s="71" t="s">
         <v>100</v>
       </c>
       <c r="L2" s="38"/>
@@ -17637,21 +16975,21 @@
       <c r="IC2" s="1"/>
     </row>
     <row r="3" spans="1:237" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="105" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="72"/>
       <c r="L3" s="38"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -17880,17 +17218,17 @@
       <c r="IC3" s="1"/>
     </row>
     <row r="4" spans="1:237" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="96"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="92"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="73"/>
       <c r="L4" s="38"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -18617,7 +17955,7 @@
         <v>135</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="E7" s="62" t="s">
         <v>146</v>
@@ -19121,10 +18459,10 @@
       <c r="IC9" s="1"/>
     </row>
     <row r="10" spans="1:237" s="9" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="71">
+      <c r="A10" s="78">
         <v>2</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="80" t="s">
         <v>104</v>
       </c>
       <c r="C10" s="109" t="s">
@@ -19374,8 +18712,8 @@
       <c r="IC10" s="13"/>
     </row>
     <row r="11" spans="1:237" s="9" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="71"/>
-      <c r="B11" s="73"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="110"/>
       <c r="D11" s="62" t="s">
         <v>149</v>
@@ -19621,8 +18959,8 @@
       <c r="IC11" s="13"/>
     </row>
     <row r="12" spans="1:237" s="9" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="110"/>
       <c r="D12" s="62" t="s">
         <v>151</v>
@@ -20643,10 +19981,10 @@
       <c r="IC17" s="1"/>
     </row>
     <row r="18" spans="1:237" s="9" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="71">
+      <c r="A18" s="78">
         <v>4</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="80" t="s">
         <v>157</v>
       </c>
       <c r="C18" s="109" t="s">
@@ -20892,8 +20230,8 @@
       <c r="IC18" s="13"/>
     </row>
     <row r="19" spans="1:237" s="9" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="110"/>
       <c r="D19" s="62" t="s">
         <v>159</v>
@@ -21150,12 +20488,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="B1:D1"/>
@@ -21166,14 +20500,18 @@
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <conditionalFormatting sqref="I8">
     <cfRule type="cellIs" priority="155" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="156" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21181,7 +20519,7 @@
     <cfRule type="cellIs" priority="153" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="154" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21189,7 +20527,7 @@
     <cfRule type="cellIs" priority="93" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="94" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21197,7 +20535,7 @@
     <cfRule type="cellIs" priority="107" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="108" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21205,7 +20543,7 @@
     <cfRule type="cellIs" priority="105" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="106" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21213,7 +20551,7 @@
     <cfRule type="cellIs" priority="103" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="104" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21221,7 +20559,7 @@
     <cfRule type="cellIs" priority="101" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="102" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21229,7 +20567,7 @@
     <cfRule type="cellIs" priority="99" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="100" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21237,7 +20575,7 @@
     <cfRule type="cellIs" priority="95" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="96" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21245,7 +20583,7 @@
     <cfRule type="cellIs" priority="91" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="92" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21253,7 +20591,7 @@
     <cfRule type="cellIs" priority="81" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="82" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21261,7 +20599,7 @@
     <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="80" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21269,7 +20607,7 @@
     <cfRule type="cellIs" priority="77" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="78" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21277,7 +20615,7 @@
     <cfRule type="cellIs" priority="75" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="76" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21285,7 +20623,7 @@
     <cfRule type="cellIs" priority="73" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="74" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21293,7 +20631,7 @@
     <cfRule type="cellIs" priority="71" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="72" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21301,7 +20639,7 @@
     <cfRule type="cellIs" priority="69" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="70" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21309,7 +20647,7 @@
     <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="68" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21317,7 +20655,7 @@
     <cfRule type="cellIs" priority="59" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="60" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21325,7 +20663,7 @@
     <cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="62" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21333,7 +20671,7 @@
     <cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="4" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21341,7 +20679,7 @@
     <cfRule type="cellIs" priority="57" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="58" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21349,7 +20687,7 @@
     <cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="16" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21357,7 +20695,7 @@
     <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="56" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21365,7 +20703,7 @@
     <cfRule type="cellIs" priority="53" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="54" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21373,7 +20711,7 @@
     <cfRule type="cellIs" priority="51" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="52" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21381,7 +20719,7 @@
     <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="50" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21389,7 +20727,7 @@
     <cfRule type="cellIs" priority="47" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="48" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21397,7 +20735,7 @@
     <cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="18" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21405,7 +20743,7 @@
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21413,7 +20751,7 @@
     <cfRule type="cellIs" priority="39" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="40" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21421,7 +20759,7 @@
     <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="38" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21429,7 +20767,7 @@
     <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21437,7 +20775,7 @@
     <cfRule type="cellIs" priority="29" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="30" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21445,7 +20783,7 @@
     <cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="28" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21453,7 +20791,7 @@
     <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="26" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21461,7 +20799,7 @@
     <cfRule type="cellIs" priority="23" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="24" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21469,7 +20807,7 @@
     <cfRule type="cellIs" priority="21" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="22" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21477,7 +20815,7 @@
     <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="20" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21485,7 +20823,7 @@
     <cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="12" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21493,7 +20831,7 @@
     <cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="10" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>